<commit_message>
- Adding random mail utility - Adding input variables
</commit_message>
<xml_diff>
--- a/src/com/generic/testdata/DataSheet.xlsx
+++ b/src/com/generic/testdata/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="17175" windowHeight="6870" activeTab="1"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="17175" windowHeight="6390" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,13 @@
     <sheet name="tmp" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="M1:Q14"/>
+  <oleSize ref="A1:K13"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="39">
   <si>
     <t>TCID</t>
   </si>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,22 +792,79 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="A3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="14">
+        <v>44122</v>
+      </c>
+      <c r="G3" s="14">
+        <v>123</v>
+      </c>
+      <c r="H3" s="14">
+        <v>123</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" spans="1:17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -815,11 +872,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="K7" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="54" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -985,9 +1045,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Change-Id: I78d4249a7cc707fb66e98f310677dcb205c84374 Signed-off-by: Ibatta <Ibatta@Ibatta-Lap>
</commit_message>
<xml_diff>
--- a/src/com/generic/testdata/DataSheet.xlsx
+++ b/src/com/generic/testdata/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="17175" windowHeight="6390"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="17175" windowHeight="6390" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,13 @@
     <sheet name="tmp" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:M16"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
   <si>
     <t>TCID</t>
   </si>
@@ -129,6 +129,60 @@
   </si>
   <si>
     <t>Accepta</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>sel_email</t>
+  </si>
+  <si>
+    <t>sel_checkEmail</t>
+  </si>
+  <si>
+    <t>sel_firstName</t>
+  </si>
+  <si>
+    <t>sel_lastName</t>
+  </si>
+  <si>
+    <t>sel_country</t>
+  </si>
+  <si>
+    <t>sel_postalCode</t>
+  </si>
+  <si>
+    <t>sel_password</t>
+  </si>
+  <si>
+    <t>sel_heckPwd</t>
+  </si>
+  <si>
+    <t>sel_createAccount</t>
+  </si>
+  <si>
+    <t>sel_email.errors</t>
+  </si>
+  <si>
+    <t>sel_checkEmail.errors</t>
+  </si>
+  <si>
+    <t>sel_firstName.errors</t>
+  </si>
+  <si>
+    <t>sel_lastName.errors</t>
+  </si>
+  <si>
+    <t>sel_country.errors</t>
+  </si>
+  <si>
+    <t>sel_postalCode.errors</t>
+  </si>
+  <si>
+    <t>sel_pwd.errors</t>
+  </si>
+  <si>
+    <t>sel_checkPwd.errors</t>
   </si>
 </sst>
 </file>
@@ -624,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,10 +720,250 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="11">
+        <v>44122</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="11"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="11">
+        <v>44122</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="11"/>
+      <c r="K3" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="14">
+        <v>44122</v>
+      </c>
+      <c r="H4" s="14">
+        <v>123</v>
+      </c>
+      <c r="I4" s="14">
+        <v>123</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R5" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q4"/>
+  <sheetViews>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,126 +1040,6 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="48.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
     <row r="2" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>11</v>

</xml_diff>